<commit_message>
68 bus time-domain complete
</commit_message>
<xml_diff>
--- a/system_cases/NETSNYPS68bus/NETS_NYPS_68_modified_detuned.xlsx
+++ b/system_cases/NETSNYPS68bus/NETS_NYPS_68_modified_detuned.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitRep\Simplus-Grid-Tool\modified_ieee_14\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitRep\Simplus-Grid-Tool\system_cases\NETSNYPS68bus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED04EC5-2B89-4761-AFBF-C06E2DDCA509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B610F142-AB33-4393-85B8-0FC60B2AD63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4860" yWindow="3970" windowWidth="28800" windowHeight="15370" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4860" yWindow="3970" windowWidth="28800" windowHeight="15370" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -3691,7 +3691,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34645F5B-1D7A-4323-9AD6-5FF81941CA24}">
   <dimension ref="A1:AQ71"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -6436,7 +6436,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D00B5E-E2E7-41B8-8388-8931D474EA96}">
   <dimension ref="A1:G88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+    <sheetView topLeftCell="A70" workbookViewId="0">
       <selection activeCell="H85" sqref="H85"/>
     </sheetView>
   </sheetViews>
@@ -8409,8 +8409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFCB373-2341-40B6-A375-7BA50357479A}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>